<commit_message>
Adelanto en el cronograma de las sesiones de diseño
</commit_message>
<xml_diff>
--- a/Crono 2019-1.xlsx
+++ b/Crono 2019-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\1143848922\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\1143848922\Documents\GIT\AplicacionesMoviles191\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -90,9 +90,6 @@
     <t>Layouts nivel 2 (ListView, GridView y RecyclerView). Georeferenciación. Ejercicio Básico Android</t>
   </si>
   <si>
-    <t>Práctico 1</t>
-  </si>
-  <si>
     <t>Firebase 2. Arquitectura de bases de datos no relaciones</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>Despliege de aplicaciones</t>
+  </si>
+  <si>
+    <t>Pitch en primeta hora de clase + Prático 1</t>
   </si>
 </sst>
 </file>
@@ -746,8 +746,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -859,7 +859,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="15.5">
+    <row r="5" spans="1:12" ht="31">
       <c r="A5" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -943,8 +943,8 @@
       <c r="C8" s="22">
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>11</v>
+      <c r="D8" s="45" t="s">
+        <v>27</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="4"/>
@@ -967,8 +967,8 @@
       <c r="C9" s="7">
         <v>2</v>
       </c>
-      <c r="D9" s="45" t="s">
-        <v>23</v>
+      <c r="D9" s="21" t="s">
+        <v>11</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="4"/>
@@ -992,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="4"/>
@@ -1016,7 +1016,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="4"/>
@@ -1040,7 +1040,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="4"/>
@@ -1180,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>18</v>

</xml_diff>